<commit_message>
add week 1 submission form for competition
</commit_message>
<xml_diff>
--- a/docs/modelling/assets/BetfairDatathonPuntingFormDataSpecifications.xlsx
+++ b/docs/modelling/assets/BetfairDatathonPuntingFormDataSpecifications.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c9c29a8f24be3a5/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motykam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0E652A-8360-49A6-8560-3E715E6D121F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11090"/>
+    <workbookView xWindow="-14190" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PF | BF Datathon Data Specs" sheetId="1" r:id="rId1"/>
@@ -456,15 +457,9 @@
     <t>Betting flucs (if available)</t>
   </si>
   <si>
-    <t>Official starting price</t>
-  </si>
-  <si>
     <t>Stewards remarks</t>
   </si>
   <si>
-    <t>Betfair Price</t>
-  </si>
-  <si>
     <t>Gear changes</t>
   </si>
   <si>
@@ -559,12 +554,18 @@
   </si>
   <si>
     <t>Beaten Margin at Finish</t>
+  </si>
+  <si>
+    <t>Betfair Starting Price (not available before the race)</t>
+  </si>
+  <si>
+    <t>Official starting price (or Pre-Post price if before the race)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -989,6 +990,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1024,6 +1042,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1199,14 +1234,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.3"/>
@@ -1218,10 +1253,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="11" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.3">
@@ -1274,18 +1309,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1573,7 +1608,7 @@
         <v>78</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -1581,7 +1616,7 @@
         <v>79</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1589,7 +1624,7 @@
         <v>80</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1597,7 +1632,7 @@
         <v>81</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1605,7 +1640,7 @@
         <v>82</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1613,7 +1648,7 @@
         <v>83</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1621,7 +1656,7 @@
         <v>84</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1629,7 +1664,7 @@
         <v>85</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1637,7 +1672,7 @@
         <v>86</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1645,7 +1680,7 @@
         <v>87</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1653,7 +1688,7 @@
         <v>88</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1661,7 +1696,7 @@
         <v>89</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1669,7 +1704,7 @@
         <v>90</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -1677,7 +1712,7 @@
         <v>91</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1685,7 +1720,7 @@
         <v>92</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="31" x14ac:dyDescent="0.3">
@@ -1693,7 +1728,7 @@
         <v>93</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="93" x14ac:dyDescent="0.3">
@@ -1765,7 +1800,7 @@
         <v>94</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="101" customHeight="1" x14ac:dyDescent="0.3">
@@ -1821,7 +1856,7 @@
         <v>95</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="31" x14ac:dyDescent="0.3">
@@ -1853,7 +1888,7 @@
         <v>96</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="31" x14ac:dyDescent="0.3">
@@ -1861,7 +1896,7 @@
         <v>97</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="31" x14ac:dyDescent="0.3">
@@ -1869,7 +1904,7 @@
         <v>98</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="31" x14ac:dyDescent="0.3">
@@ -1877,7 +1912,7 @@
         <v>99</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="31" x14ac:dyDescent="0.3">
@@ -1885,7 +1920,7 @@
         <v>100</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1893,7 +1928,7 @@
         <v>101</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="31" x14ac:dyDescent="0.3">
@@ -1901,7 +1936,7 @@
         <v>102</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="31" x14ac:dyDescent="0.3">
@@ -1909,7 +1944,7 @@
         <v>103</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="31" x14ac:dyDescent="0.3">
@@ -1917,7 +1952,7 @@
         <v>104</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="31" x14ac:dyDescent="0.3">
@@ -1925,7 +1960,7 @@
         <v>105</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="31" x14ac:dyDescent="0.3">
@@ -1933,7 +1968,7 @@
         <v>106</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>